<commit_message>
ajout résultats + run finaux
</commit_message>
<xml_diff>
--- a/sensibilite_CO2_cost.xlsx
+++ b/sensibilite_CO2_cost.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\augus\cours-ensta\EA\Projet-EA314\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4229AE36-19F7-4E59-AEE5-D9B222750751}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{805332FF-4363-4D90-8907-695A849D23BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="000 Cost Data" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,12 @@
     <sheet name="1000 Capacity Data" sheetId="10" r:id="rId10"/>
     <sheet name="1000 Optimised Cost" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="26">
   <si>
     <t>unserved_energy_cost</t>
   </si>
@@ -567,6 +567,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.7265625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" s="1">
@@ -630,9 +633,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.453125" customWidth="1"/>
+    <col min="2" max="2" width="19.90625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" s="1">
@@ -716,8 +725,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.54296875" customWidth="1"/>
-    <col min="2" max="2" width="12.54296875" customWidth="1"/>
+    <col min="1" max="1" width="18.54296875" customWidth="1"/>
+    <col min="2" max="2" width="19.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -780,82 +789,146 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="13.54296875" customWidth="1"/>
+    <col min="1" max="1" width="19.1796875" customWidth="1"/>
+    <col min="2" max="2" width="18.6328125" customWidth="1"/>
+    <col min="6" max="6" width="7.6328125" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="8" max="8" width="14.36328125" customWidth="1"/>
+    <col min="9" max="9" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="I1" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B2">
         <v>228.72555668148479</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="H2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2">
+        <v>309.65881936780858</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B3">
         <v>76.932508737294228</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="H3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3">
+        <v>197.7095904561954</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B4">
         <v>3.9882153687500002</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="H4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4">
+        <v>6.1401243242399994</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B5">
         <v>7.9663496675142191</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="H5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5">
+        <v>2.7989271163314511</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B6">
         <v>0.22786256760339979</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="H6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6">
+        <v>4.5637878177599997E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B7">
         <v>140.7869362016186</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="H7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7">
+        <v>190.6036084429094</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B8">
         <v>34.610863809708668</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="H8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8">
+        <v>12.16031046586941</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B9">
         <v>34610.863809708673</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9">
+        <v>12160.31046586941</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G12">
+        <f>(I2-B2)/(I9-B9)*1000</f>
+        <v>-3.6049562541643536</v>
       </c>
     </row>
   </sheetData>
@@ -870,6 +943,10 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.54296875" customWidth="1"/>
+    <col min="2" max="2" width="17.6328125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" s="1">
@@ -933,11 +1010,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23.08984375" customWidth="1"/>
+    <col min="2" max="2" width="15.81640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" s="1">
@@ -1017,9 +1098,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.1796875" customWidth="1"/>
+    <col min="2" max="2" width="14.08984375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" s="1">

</xml_diff>